<commit_message>
#3456 updated PM Property ID
</commit_message>
<xml_diff>
--- a/seed/tests/data/CBL-building-performance-standards-sample-2019.xlsx
+++ b/seed/tests/data/CBL-building-performance-standards-sample-2019.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achapin/seed/seed/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB2F19D-0315-8A40-A3A3-D5589C32F5CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB934BB-CEDF-664F-AF69-921CE78991DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="11000" windowWidth="35840" windowHeight="10480" xr2:uid="{ABA70866-58E3-E741-9E6E-8CBE8BD4F008}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20980" xr2:uid="{ABA70866-58E3-E741-9E6E-8CBE8BD4F008}"/>
   </bookViews>
   <sheets>
     <sheet name="BPS Data" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -607,7 +607,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="B16" sqref="B16:C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -662,7 +662,7 @@
         <v>11911</v>
       </c>
       <c r="B2">
-        <v>21537666</v>
+        <v>22178843</v>
       </c>
       <c r="C2" t="s">
         <v>14</v>
@@ -703,7 +703,7 @@
         <v>12227</v>
       </c>
       <c r="B3">
-        <v>21537667</v>
+        <v>22178844</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -744,7 +744,7 @@
         <v>17971</v>
       </c>
       <c r="B4">
-        <v>21537668</v>
+        <v>22178845</v>
       </c>
       <c r="C4" t="s">
         <v>25</v>
@@ -785,7 +785,7 @@
         <v>21381</v>
       </c>
       <c r="B5">
-        <v>21537669</v>
+        <v>22178846</v>
       </c>
       <c r="C5" t="s">
         <v>29</v>
@@ -826,7 +826,7 @@
         <v>21404</v>
       </c>
       <c r="B6">
-        <v>21537670</v>
+        <v>22178847</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -867,7 +867,7 @@
         <v>21405</v>
       </c>
       <c r="B7">
-        <v>21537671</v>
+        <v>22178848</v>
       </c>
       <c r="C7" t="s">
         <v>38</v>
@@ -908,7 +908,7 @@
         <v>21368</v>
       </c>
       <c r="B8">
-        <v>21537672</v>
+        <v>22178849</v>
       </c>
       <c r="C8" t="s">
         <v>42</v>
@@ -949,7 +949,7 @@
         <v>21378</v>
       </c>
       <c r="B9">
-        <v>21537673</v>
+        <v>22178850</v>
       </c>
       <c r="C9" t="s">
         <v>46</v>
@@ -990,7 +990,7 @@
         <v>21426</v>
       </c>
       <c r="B10">
-        <v>21537674</v>
+        <v>22178851</v>
       </c>
       <c r="C10" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
#3473 replaced two properties that had gaps
</commit_message>
<xml_diff>
--- a/seed/tests/data/CBL-building-performance-standards-sample-2019.xlsx
+++ b/seed/tests/data/CBL-building-performance-standards-sample-2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achapin/seed/seed/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBB934BB-CEDF-664F-AF69-921CE78991DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C7B78C-AA6C-794F-9D2A-9C8D97ED147B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20980" xr2:uid="{ABA70866-58E3-E741-9E6E-8CBE8BD4F008}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20180" xr2:uid="{ABA70866-58E3-E741-9E6E-8CBE8BD4F008}"/>
   </bookViews>
   <sheets>
     <sheet name="BPS Data" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>Property Name</t>
   </si>
@@ -46,9 +46,6 @@
     <t>Medical Office</t>
   </si>
   <si>
-    <t>EUI Target Year</t>
-  </si>
-  <si>
     <t>Audit Template Building ID</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
     <t>Gross Area (SF)</t>
   </si>
   <si>
-    <t>Medstar POB North Tower</t>
-  </si>
-  <si>
     <t>106 IRVING ST NW</t>
   </si>
   <si>
@@ -97,9 +91,6 @@
     <t>admin@companya.com</t>
   </si>
   <si>
-    <t>1801 Pennsylvania Ave.</t>
-  </si>
-  <si>
     <t>Office</t>
   </si>
   <si>
@@ -115,12 +106,6 @@
     <t>GSA: 300 E Street SW</t>
   </si>
   <si>
-    <t>0300 E ST SW</t>
-  </si>
-  <si>
-    <t>WELLS REIT/INDEPENDENCE SQUARE LLC</t>
-  </si>
-  <si>
     <t>admin@companyc.com</t>
   </si>
   <si>
@@ -136,18 +121,9 @@
     <t>admin@companyd.com</t>
   </si>
   <si>
-    <t>President Madison Apartments</t>
-  </si>
-  <si>
     <t>Multifamily</t>
   </si>
   <si>
-    <t>1908 FLORIDA AV NW</t>
-  </si>
-  <si>
-    <t>BDC PRESIDENT MADISON LLC</t>
-  </si>
-  <si>
     <t>admin@companye.com</t>
   </si>
   <si>
@@ -166,9 +142,6 @@
     <t>15th and H Street Associates LLP</t>
   </si>
   <si>
-    <t>733 15TH ST NW</t>
-  </si>
-  <si>
     <t>15TH AND H STREET ASSOCIATES LP</t>
   </si>
   <si>
@@ -190,19 +163,40 @@
     <t>admin@companyh.com</t>
   </si>
   <si>
-    <t>DPW Vehicle Maintenance Facility 2</t>
-  </si>
-  <si>
-    <t>Service-Repair</t>
-  </si>
-  <si>
-    <t>1242  MOUNT OLIVET RD NE</t>
-  </si>
-  <si>
-    <t>GOVERNMENT OF THE DISTRICT OF COLUMBIA DEPARTMENT OF GENERAL SERVICES</t>
-  </si>
-  <si>
     <t>admin@companyi.com</t>
+  </si>
+  <si>
+    <t>Medstar POB South Tower</t>
+  </si>
+  <si>
+    <t>1801 Pennsylvania Avenue, LLC</t>
+  </si>
+  <si>
+    <t>300 E ST SW</t>
+  </si>
+  <si>
+    <t>TWO INDEPENDENCE HANA OW LLC</t>
+  </si>
+  <si>
+    <t>Hampton House</t>
+  </si>
+  <si>
+    <t>2700 CONNECTICUT AVENUE NW</t>
+  </si>
+  <si>
+    <t>2700 CONECTICUT AVENUE LLC</t>
+  </si>
+  <si>
+    <t>1428 H ST NW</t>
+  </si>
+  <si>
+    <t>School Without Walls @ Francis Stevens</t>
+  </si>
+  <si>
+    <t>K-12 School</t>
+  </si>
+  <si>
+    <t>2425 N STREET NW</t>
   </si>
 </sst>
 </file>
@@ -281,13 +275,12 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -604,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14AAF8DA-FAFC-5247-8BBA-26096DB3751B}">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:C24"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -616,12 +609,12 @@
     <col min="9" max="9" width="18.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>0</v>
@@ -630,34 +623,31 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="M1" t="s">
-        <v>3</v>
-      </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>11911</v>
       </c>
@@ -665,40 +655,37 @@
         <v>22178843</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
       <c r="D2" t="s">
         <v>2</v>
       </c>
       <c r="E2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
         <v>15</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
       </c>
       <c r="H2">
         <v>20010</v>
       </c>
       <c r="I2">
-        <v>1967</v>
+        <v>1985</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="K2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="L2">
-        <v>106517</v>
-      </c>
-      <c r="M2">
-        <v>2020</v>
+        <v>76319</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>12227</v>
       </c>
@@ -706,19 +693,19 @@
         <v>22178844</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H3">
         <v>20006</v>
@@ -727,19 +714,16 @@
         <v>1991</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="L3">
         <v>220131</v>
       </c>
-      <c r="M3">
-        <v>2020</v>
-      </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>17971</v>
       </c>
@@ -747,19 +731,19 @@
         <v>22178845</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H4">
         <v>20546</v>
@@ -768,19 +752,16 @@
         <v>1991</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="K4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="L4">
-        <v>659773</v>
-      </c>
-      <c r="M4">
-        <v>2020</v>
+        <v>627655</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>21381</v>
       </c>
@@ -788,19 +769,19 @@
         <v>22178846</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H5">
         <v>20036</v>
@@ -809,19 +790,16 @@
         <v>1962</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="K5" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="L5">
-        <v>65273</v>
-      </c>
-      <c r="M5">
-        <v>2020</v>
+        <v>58717</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>21404</v>
       </c>
@@ -829,40 +807,37 @@
         <v>22178847</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>47</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H6">
-        <v>20009</v>
+        <v>20008</v>
       </c>
       <c r="I6">
-        <v>1908</v>
+        <v>1921</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="K6" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="L6">
-        <v>86166</v>
-      </c>
-      <c r="M6">
-        <v>2020</v>
+        <v>83580</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>21405</v>
       </c>
@@ -870,40 +845,37 @@
         <v>22178848</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="F7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G7" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H7">
-        <v>20007</v>
+        <v>20005</v>
       </c>
       <c r="I7">
         <v>2004</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="K7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="L7">
-        <v>134036</v>
-      </c>
-      <c r="M7">
-        <v>2020</v>
+        <v>145697</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>21368</v>
       </c>
@@ -911,19 +883,19 @@
         <v>22178849</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E8" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H8">
         <v>20005</v>
@@ -932,19 +904,16 @@
         <v>1912</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="K8" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="L8">
         <v>230129</v>
       </c>
-      <c r="M8">
-        <v>2020</v>
-      </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>21378</v>
       </c>
@@ -952,19 +921,19 @@
         <v>22178850</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D9" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="E9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="F9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H9">
         <v>20003</v>
@@ -973,19 +942,16 @@
         <v>1880</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="K9" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="L9">
         <v>29906</v>
       </c>
-      <c r="M9">
-        <v>2020</v>
-      </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>21426</v>
       </c>
@@ -1002,28 +968,25 @@
         <v>53</v>
       </c>
       <c r="F10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="H10">
-        <v>20002</v>
-      </c>
-      <c r="I10" s="3">
-        <v>1952</v>
+        <v>20037</v>
+      </c>
+      <c r="I10">
+        <v>1924</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>54</v>
+        <v>40</v>
       </c>
       <c r="K10" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="L10">
-        <v>134114</v>
-      </c>
-      <c r="M10">
-        <v>2020</v>
+        <v>127991</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#3473 swapped out two properties
</commit_message>
<xml_diff>
--- a/seed/tests/data/CBL-building-performance-standards-sample-2019.xlsx
+++ b/seed/tests/data/CBL-building-performance-standards-sample-2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/achapin/seed/seed/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48C7B78C-AA6C-794F-9D2A-9C8D97ED147B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9E90D9D-8C66-E349-A89E-D42A522D9A5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20180" xr2:uid="{ABA70866-58E3-E741-9E6E-8CBE8BD4F008}"/>
+    <workbookView xWindow="38420" yWindow="1640" windowWidth="21600" windowHeight="20180" xr2:uid="{ABA70866-58E3-E741-9E6E-8CBE8BD4F008}"/>
   </bookViews>
   <sheets>
     <sheet name="BPS Data" sheetId="2" r:id="rId1"/>
@@ -600,7 +600,7 @@
   <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="L2" sqref="L2:L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -758,7 +758,7 @@
         <v>23</v>
       </c>
       <c r="L4">
-        <v>627655</v>
+        <v>659773</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
@@ -804,7 +804,7 @@
         <v>21404</v>
       </c>
       <c r="B6">
-        <v>22178847</v>
+        <v>22482006</v>
       </c>
       <c r="C6" t="s">
         <v>47</v>
@@ -872,7 +872,7 @@
         <v>33</v>
       </c>
       <c r="L7">
-        <v>145697</v>
+        <v>134036</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.2">
@@ -956,7 +956,7 @@
         <v>21426</v>
       </c>
       <c r="B10">
-        <v>22178851</v>
+        <v>22482007</v>
       </c>
       <c r="C10" t="s">
         <v>51</v>

</xml_diff>